<commit_message>
fixed NHIS district code error
</commit_message>
<xml_diff>
--- a/health/sigungu_nhis.xlsx
+++ b/health/sigungu_nhis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/91bb9e7cfb03414a/SNU/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:40009_{C9236FC5-D5D3-4BDC-9042-2CBEECEB9D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C5E4C35-648B-4153-8535-18CED00493F6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301055E3-AD48-4631-8218-2174FDBD7F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3456" windowWidth="28620" windowHeight="17340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23470" yWindow="-1570" windowWidth="34340" windowHeight="20810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cleaned" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2111" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2110" uniqueCount="380">
   <si>
     <t>행정구역분류코드</t>
   </si>
@@ -2138,8 +2138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G265"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="E120" sqref="E120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -4077,9 +4077,6 @@
       <c r="F85" t="s">
         <v>284</v>
       </c>
-      <c r="G85" t="s">
-        <v>236</v>
-      </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A86">
@@ -4101,7 +4098,7 @@
         <v>284</v>
       </c>
       <c r="G86" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.4">
@@ -4124,7 +4121,7 @@
         <v>290</v>
       </c>
       <c r="G87" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.4">
@@ -4147,7 +4144,7 @@
         <v>290</v>
       </c>
       <c r="G88" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.4">
@@ -4170,7 +4167,7 @@
         <v>290</v>
       </c>
       <c r="G89" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.4">
@@ -4193,7 +4190,7 @@
         <v>290</v>
       </c>
       <c r="G90" t="s">
-        <v>215</v>
+        <v>250</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.4">
@@ -4216,7 +4213,7 @@
         <v>290</v>
       </c>
       <c r="G91" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.4">
@@ -4239,7 +4236,7 @@
         <v>290</v>
       </c>
       <c r="G92" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.4">
@@ -4262,7 +4259,7 @@
         <v>290</v>
       </c>
       <c r="G93" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.4">
@@ -4285,7 +4282,7 @@
         <v>290</v>
       </c>
       <c r="G94" t="s">
-        <v>56</v>
+        <v>210</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.4">

</xml_diff>